<commit_message>
make the flags default for templates
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.10.xlsx
+++ b/schema_definitions/template_schema_v1.10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ala/Desktop/workspace/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8694A0DC-D13A-9549-A11E-7E8088B7D2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB092C8-BA4F-B041-959E-AB3126F58CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3400" yWindow="900" windowWidth="28800" windowHeight="17500" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2019,7 +2019,7 @@
         <v>193</v>
       </c>
       <c r="C23" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="5" t="b">
         <v>0</v>
@@ -2063,7 +2063,7 @@
         <v>194</v>
       </c>
       <c r="C24" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5" t="b">
         <v>0</v>
@@ -2107,7 +2107,7 @@
         <v>195</v>
       </c>
       <c r="C25" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5" t="b">
         <v>0</v>

</xml_diff>